<commit_message>
Section 3_Testing Documentation & Test Case & Tracking Management Tools
</commit_message>
<xml_diff>
--- a/3_Testing Documentation & Test Case & Tracking Management Tools/Praktikum/Tugas Testing Documentation (Soal Prioritas 1 - Soal Prioritas 2).xlsx
+++ b/3_Testing Documentation & Test Case & Tracking Management Tools/Praktikum/Tugas Testing Documentation (Soal Prioritas 1 - Soal Prioritas 2).xlsx
@@ -1148,7 +1148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1193,7 +1193,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1249,15 +1248,105 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1271,143 +1360,89 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1621,8 +1656,8 @@
   </sheetPr>
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63:G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1697,50 +1732,50 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="55"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56" t="s">
+      <c r="E5" s="85"/>
+      <c r="F5" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="58"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="91"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="59" t="s">
+      <c r="E6" s="85"/>
+      <c r="F6" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="60" t="s">
+      <c r="G6" s="91"/>
+      <c r="H6" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62" t="s">
+      <c r="I6" s="100"/>
+      <c r="J6" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="58"/>
+      <c r="K6" s="91"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="A7" s="6"/>
@@ -1756,14 +1791,14 @@
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="91"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1784,36 +1819,36 @@
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="55"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="64">
+      <c r="E10" s="85"/>
+      <c r="F10" s="90">
         <v>44985</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="65" t="s">
+      <c r="G10" s="91"/>
+      <c r="H10" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="55"/>
-      <c r="J10" s="66" t="s">
+      <c r="I10" s="85"/>
+      <c r="J10" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="58"/>
+      <c r="K10" s="91"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="78"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="80"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1822,125 +1857,125 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="81" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="68"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="81" t="s">
+      <c r="F12" s="76"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="81" t="s">
+      <c r="I12" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="81" t="s">
+      <c r="J12" s="87" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="75"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="89" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="E14" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="74" t="s">
+      <c r="F14" s="76"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="100" t="s">
+      <c r="I14" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="82" t="s">
+      <c r="J14" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="118"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="77" t="s">
+      <c r="A15" s="73"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="78"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A16" s="118"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="11" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="118"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="118"/>
-      <c r="B18" s="117" t="s">
+      <c r="A18" s="73"/>
+      <c r="B18" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="89" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="83" t="s">
@@ -1951,68 +1986,68 @@
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="74" t="s">
+      <c r="H18" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="100" t="s">
+      <c r="I18" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="82" t="s">
+      <c r="J18" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A19" s="118"/>
-      <c r="B19" s="79"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="55"/>
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="118"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="19" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="20"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="118"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
       <c r="E21" s="21" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="23"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="118"/>
-      <c r="B22" s="117" t="s">
+      <c r="A22" s="73"/>
+      <c r="B22" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="80" t="s">
+      <c r="C22" s="89" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="83" t="s">
@@ -2023,68 +2058,68 @@
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="26"/>
-      <c r="H22" s="74" t="s">
+      <c r="H22" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="100" t="s">
+      <c r="I22" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="82" t="s">
+      <c r="J22" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="118"/>
-      <c r="B23" s="79"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="12"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="118"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="11" t="s">
         <v>43</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="12"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="118"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
       <c r="E25" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="118"/>
-      <c r="B26" s="117" t="s">
+      <c r="A26" s="73"/>
+      <c r="B26" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="80" t="s">
+      <c r="C26" s="89" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="83" t="s">
@@ -2095,68 +2130,68 @@
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="74" t="s">
+      <c r="H26" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="100" t="s">
+      <c r="I26" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="82" t="s">
+      <c r="J26" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="118"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="28" t="s">
         <v>31</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="20"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="55"/>
       <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="118"/>
-      <c r="B28" s="79"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="28" t="s">
         <v>46</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="20"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
       <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="118"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
       <c r="E29" s="29" t="s">
         <v>33</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="23"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="76"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="118"/>
-      <c r="B30" s="117" t="s">
+      <c r="A30" s="73"/>
+      <c r="B30" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="80" t="s">
+      <c r="C30" s="89" t="s">
         <v>47</v>
       </c>
       <c r="D30" s="83" t="s">
@@ -2167,68 +2202,68 @@
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
-      <c r="H30" s="74" t="s">
+      <c r="H30" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="100" t="s">
+      <c r="I30" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="82" t="s">
+      <c r="J30" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="118"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
       <c r="E31" s="28" t="s">
         <v>42</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="20"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
       <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="118"/>
-      <c r="B32" s="79"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
       <c r="E32" s="28" t="s">
         <v>49</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="118"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
       <c r="E33" s="29" t="s">
         <v>33</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="23"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="76"/>
-      <c r="J33" s="76"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
       <c r="K33" s="9"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="118"/>
-      <c r="B34" s="117" t="s">
+      <c r="A34" s="73"/>
+      <c r="B34" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="80" t="s">
+      <c r="C34" s="89" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="83" t="s">
@@ -2239,68 +2274,68 @@
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
-      <c r="H34" s="74" t="s">
+      <c r="H34" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="I34" s="100" t="s">
+      <c r="I34" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="82" t="s">
+      <c r="J34" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="9"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="118"/>
-      <c r="B35" s="79"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="19" t="s">
         <v>52</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="20"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="75"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
       <c r="K35" s="9"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="118"/>
-      <c r="B36" s="79"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="75"/>
+      <c r="A36" s="73"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="19" t="s">
         <v>32</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="20"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="75"/>
-      <c r="J36" s="75"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
       <c r="K36" s="9"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="118"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
       <c r="E37" s="21" t="s">
         <v>33</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="23"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="76"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
       <c r="K37" s="9"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="118"/>
-      <c r="B38" s="117" t="s">
+      <c r="A38" s="73"/>
+      <c r="B38" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="80" t="s">
+      <c r="C38" s="89" t="s">
         <v>53</v>
       </c>
       <c r="D38" s="83" t="s">
@@ -2311,68 +2346,68 @@
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
-      <c r="H38" s="74" t="s">
+      <c r="H38" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="I38" s="100" t="s">
+      <c r="I38" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J38" s="82" t="s">
+      <c r="J38" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="118"/>
-      <c r="B39" s="79"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
+      <c r="A39" s="73"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
       <c r="E39" s="19" t="s">
         <v>55</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="20"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="75"/>
-      <c r="J39" s="75"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
       <c r="K39" s="9"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A40" s="118"/>
-      <c r="B40" s="79"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
       <c r="E40" s="19" t="s">
         <v>32</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="20"/>
-      <c r="H40" s="75"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
       <c r="K40" s="9"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A41" s="118"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
       <c r="E41" s="21" t="s">
         <v>33</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="23"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
       <c r="K41" s="9"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="118"/>
-      <c r="B42" s="117" t="s">
+      <c r="A42" s="73"/>
+      <c r="B42" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="84" t="s">
+      <c r="C42" s="82" t="s">
         <v>56</v>
       </c>
       <c r="D42" s="83" t="s">
@@ -2383,64 +2418,64 @@
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="74" t="s">
+      <c r="H42" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="I42" s="100" t="s">
+      <c r="I42" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J42" s="82" t="s">
+      <c r="J42" s="63" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="9"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="118"/>
-      <c r="B43" s="79"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="75"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
       <c r="E43" s="19" t="s">
         <v>58</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="20"/>
-      <c r="H43" s="75"/>
-      <c r="I43" s="75"/>
-      <c r="J43" s="75"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="118"/>
-      <c r="B44" s="79"/>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
+      <c r="A44" s="73"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
       <c r="E44" s="19" t="s">
         <v>32</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="20"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="75"/>
-      <c r="J44" s="75"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A45" s="118"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="21" t="s">
         <v>33</v>
       </c>
       <c r="F45" s="22"/>
       <c r="G45" s="23"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="76"/>
-      <c r="J45" s="76"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A46" s="119"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
@@ -2453,627 +2488,730 @@
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="86" t="s">
+      <c r="A47" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="87" t="s">
+      <c r="B47" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="69"/>
-      <c r="D47" s="86" t="s">
+      <c r="C47" s="75"/>
+      <c r="D47" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="E47" s="87" t="s">
+      <c r="E47" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="F47" s="68"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="86" t="s">
+      <c r="F47" s="76"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="I47" s="86" t="s">
+      <c r="I47" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="J47" s="86" t="s">
+      <c r="J47" s="58" t="s">
         <v>23</v>
       </c>
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A48" s="76"/>
-      <c r="B48" s="70"/>
-      <c r="C48" s="72"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="72"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="76"/>
-      <c r="J48" s="76"/>
+      <c r="A48" s="56"/>
+      <c r="B48" s="68"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="68"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A49" s="94" t="s">
+      <c r="A49" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="90" t="s">
+      <c r="B49" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="91" t="s">
+      <c r="C49" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="92" t="s">
+      <c r="D49" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="E49" s="88" t="s">
+      <c r="E49" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="F49" s="68"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="98" t="s">
+      <c r="F49" s="76"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="I49" s="96" t="s">
+      <c r="I49" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="J49" s="97" t="s">
+      <c r="J49" s="57" t="s">
         <v>17</v>
       </c>
       <c r="K49" s="9"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A50" s="75"/>
-      <c r="B50" s="75"/>
-      <c r="C50" s="75"/>
-      <c r="D50" s="93"/>
-      <c r="E50" s="89" t="s">
+      <c r="A50" s="55"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F50" s="78"/>
-      <c r="G50" s="79"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="75"/>
-      <c r="J50" s="75"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="55"/>
       <c r="K50" s="9"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A51" s="75"/>
-      <c r="B51" s="75"/>
-      <c r="C51" s="75"/>
-      <c r="D51" s="93"/>
+      <c r="A51" s="55"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="67"/>
       <c r="E51" s="28" t="s">
         <v>65</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="20"/>
-      <c r="H51" s="79"/>
-      <c r="I51" s="75"/>
-      <c r="J51" s="75"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="55"/>
       <c r="K51" s="9"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A52" s="75"/>
-      <c r="B52" s="75"/>
-      <c r="C52" s="75"/>
-      <c r="D52" s="93"/>
+      <c r="A52" s="55"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="67"/>
       <c r="E52" s="28" t="s">
         <v>66</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="20"/>
-      <c r="H52" s="79"/>
-      <c r="I52" s="75"/>
-      <c r="J52" s="75"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="55"/>
+      <c r="J52" s="55"/>
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A53" s="75"/>
-      <c r="B53" s="75"/>
-      <c r="C53" s="75"/>
-      <c r="D53" s="93"/>
+      <c r="A53" s="55"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="67"/>
       <c r="E53" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="20"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="75"/>
-      <c r="J53" s="75"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
       <c r="K53" s="9"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A54" s="75"/>
-      <c r="B54" s="76"/>
-      <c r="C54" s="76"/>
-      <c r="D54" s="70"/>
+      <c r="A54" s="55"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="68"/>
       <c r="E54" s="29" t="s">
         <v>68</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="23"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="76"/>
-      <c r="J54" s="76"/>
+      <c r="H54" s="61"/>
+      <c r="I54" s="56"/>
+      <c r="J54" s="56"/>
       <c r="K54" s="9"/>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A55" s="75"/>
-      <c r="B55" s="90" t="s">
+      <c r="A55" s="55"/>
+      <c r="B55" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="91" t="s">
+      <c r="C55" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="D55" s="95" t="s">
+      <c r="D55" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="E55" s="88" t="s">
+      <c r="E55" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="F55" s="68"/>
-      <c r="G55" s="69"/>
-      <c r="H55" s="98" t="s">
+      <c r="F55" s="76"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="I55" s="96" t="s">
+      <c r="I55" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="J55" s="97" t="s">
+      <c r="J55" s="57" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A56" s="75"/>
-      <c r="B56" s="75"/>
-      <c r="C56" s="75"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="89" t="s">
+      <c r="A56" s="55"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="78"/>
-      <c r="G56" s="79"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="75"/>
-      <c r="J56" s="75"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A57" s="75"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
+      <c r="A57" s="55"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
       <c r="E57" s="28" t="s">
         <v>70</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="20"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
+      <c r="H57" s="60"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A58" s="75"/>
-      <c r="B58" s="75"/>
-      <c r="C58" s="75"/>
-      <c r="D58" s="75"/>
+      <c r="A58" s="55"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
       <c r="E58" s="28" t="s">
         <v>66</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="20"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="75"/>
-      <c r="J58" s="75"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="55"/>
+      <c r="J58" s="55"/>
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A59" s="75"/>
-      <c r="B59" s="75"/>
-      <c r="C59" s="75"/>
-      <c r="D59" s="75"/>
+      <c r="A59" s="55"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="55"/>
       <c r="E59" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="20"/>
-      <c r="H59" s="79"/>
-      <c r="I59" s="75"/>
-      <c r="J59" s="75"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="55"/>
+      <c r="J59" s="55"/>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A60" s="75"/>
-      <c r="B60" s="76"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
+      <c r="A60" s="55"/>
+      <c r="B60" s="56"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="56"/>
       <c r="E60" s="28" t="s">
         <v>68</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="20"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="76"/>
-      <c r="J60" s="76"/>
+      <c r="H60" s="61"/>
+      <c r="I60" s="56"/>
+      <c r="J60" s="56"/>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A61" s="75"/>
-      <c r="B61" s="90" t="s">
+      <c r="A61" s="55"/>
+      <c r="B61" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="91" t="s">
+      <c r="C61" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="D61" s="92" t="s">
+      <c r="D61" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="E61" s="88" t="s">
+      <c r="E61" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="F61" s="68"/>
-      <c r="G61" s="69"/>
-      <c r="H61" s="98" t="s">
+      <c r="F61" s="76"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="I61" s="96" t="s">
+      <c r="I61" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="J61" s="97" t="s">
+      <c r="J61" s="57" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A62" s="75"/>
-      <c r="B62" s="75"/>
-      <c r="C62" s="75"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="89" t="s">
+      <c r="A62" s="55"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F62" s="78"/>
-      <c r="G62" s="79"/>
-      <c r="H62" s="79"/>
-      <c r="I62" s="75"/>
-      <c r="J62" s="75"/>
+      <c r="F62" s="80"/>
+      <c r="G62" s="60"/>
+      <c r="H62" s="60"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
     </row>
     <row r="63" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A63" s="75"/>
-      <c r="B63" s="75"/>
-      <c r="C63" s="75"/>
-      <c r="D63" s="93"/>
-      <c r="E63" s="28" t="s">
+      <c r="A63" s="55"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="55"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="79"/>
-      <c r="I63" s="75"/>
-      <c r="J63" s="75"/>
+      <c r="F63" s="129"/>
+      <c r="G63" s="130"/>
+      <c r="H63" s="60"/>
+      <c r="I63" s="55"/>
+      <c r="J63" s="55"/>
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A64" s="75"/>
-      <c r="B64" s="75"/>
-      <c r="C64" s="75"/>
-      <c r="D64" s="93"/>
-      <c r="E64" s="28" t="s">
+      <c r="A64" s="55"/>
+      <c r="B64" s="55"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="F64" s="9"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="79"/>
-      <c r="I64" s="75"/>
-      <c r="J64" s="75"/>
+      <c r="F64" s="129"/>
+      <c r="G64" s="130"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="55"/>
+      <c r="J64" s="55"/>
     </row>
     <row r="65" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A65" s="75"/>
-      <c r="B65" s="75"/>
-      <c r="C65" s="75"/>
-      <c r="D65" s="93"/>
-      <c r="E65" s="28" t="s">
+      <c r="A65" s="55"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="F65" s="9"/>
-      <c r="G65" s="20"/>
-      <c r="H65" s="79"/>
-      <c r="I65" s="75"/>
-      <c r="J65" s="75"/>
+      <c r="F65" s="129"/>
+      <c r="G65" s="130"/>
+      <c r="H65" s="60"/>
+      <c r="I65" s="55"/>
+      <c r="J65" s="55"/>
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A66" s="75"/>
-      <c r="B66" s="76"/>
-      <c r="C66" s="76"/>
-      <c r="D66" s="70"/>
-      <c r="E66" s="29" t="s">
+      <c r="A66" s="55"/>
+      <c r="B66" s="56"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="F66" s="22"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="72"/>
-      <c r="I66" s="76"/>
-      <c r="J66" s="76"/>
+      <c r="F66" s="126"/>
+      <c r="G66" s="127"/>
+      <c r="H66" s="61"/>
+      <c r="I66" s="56"/>
+      <c r="J66" s="56"/>
     </row>
     <row r="67" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A67" s="75"/>
-      <c r="B67" s="90" t="s">
+      <c r="A67" s="55"/>
+      <c r="B67" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C67" s="91" t="s">
+      <c r="C67" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="D67" s="92" t="s">
+      <c r="D67" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="E67" s="88" t="s">
+      <c r="E67" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="F67" s="68"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="99" t="s">
+      <c r="F67" s="76"/>
+      <c r="G67" s="75"/>
+      <c r="H67" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="I67" s="96" t="s">
+      <c r="I67" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="J67" s="97" t="s">
+      <c r="J67" s="57" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A68" s="75"/>
-      <c r="B68" s="75"/>
-      <c r="C68" s="75"/>
-      <c r="D68" s="93"/>
-      <c r="E68" s="89" t="s">
+      <c r="A68" s="55"/>
+      <c r="B68" s="55"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="F68" s="78"/>
-      <c r="G68" s="79"/>
-      <c r="H68" s="79"/>
-      <c r="I68" s="75"/>
-      <c r="J68" s="75"/>
+      <c r="F68" s="80"/>
+      <c r="G68" s="60"/>
+      <c r="H68" s="60"/>
+      <c r="I68" s="55"/>
+      <c r="J68" s="55"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A69" s="75"/>
-      <c r="B69" s="75"/>
-      <c r="C69" s="75"/>
-      <c r="D69" s="93"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="20"/>
-      <c r="H69" s="79"/>
-      <c r="I69" s="75"/>
-      <c r="J69" s="75"/>
+      <c r="A69" s="55"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="119"/>
+      <c r="F69" s="120"/>
+      <c r="G69" s="121"/>
+      <c r="H69" s="60"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="55"/>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A70" s="75"/>
-      <c r="B70" s="75"/>
-      <c r="C70" s="75"/>
-      <c r="D70" s="93"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="79"/>
-      <c r="I70" s="75"/>
-      <c r="J70" s="75"/>
+      <c r="A70" s="55"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="119"/>
+      <c r="F70" s="120"/>
+      <c r="G70" s="121"/>
+      <c r="H70" s="60"/>
+      <c r="I70" s="55"/>
+      <c r="J70" s="55"/>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A71" s="75"/>
-      <c r="B71" s="75"/>
-      <c r="C71" s="75"/>
-      <c r="D71" s="93"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="79"/>
-      <c r="I71" s="75"/>
-      <c r="J71" s="75"/>
+      <c r="A71" s="55"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="120"/>
+      <c r="G71" s="121"/>
+      <c r="H71" s="60"/>
+      <c r="I71" s="55"/>
+      <c r="J71" s="55"/>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A72" s="75"/>
-      <c r="B72" s="76"/>
-      <c r="C72" s="76"/>
-      <c r="D72" s="70"/>
-      <c r="E72" s="30"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="76"/>
-      <c r="J72" s="76"/>
+      <c r="A72" s="55"/>
+      <c r="B72" s="56"/>
+      <c r="C72" s="56"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="122"/>
+      <c r="F72" s="123"/>
+      <c r="G72" s="124"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="56"/>
+      <c r="J72" s="56"/>
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A73" s="75"/>
-      <c r="B73" s="90" t="s">
+      <c r="A73" s="55"/>
+      <c r="B73" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C73" s="91" t="s">
+      <c r="C73" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="D73" s="92" t="s">
+      <c r="D73" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="E73" s="88" t="s">
+      <c r="E73" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="F73" s="68"/>
-      <c r="G73" s="69"/>
-      <c r="H73" s="98" t="s">
+      <c r="F73" s="76"/>
+      <c r="G73" s="75"/>
+      <c r="H73" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="I73" s="96" t="s">
+      <c r="I73" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="J73" s="97" t="s">
+      <c r="J73" s="57" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A74" s="75"/>
-      <c r="B74" s="75"/>
-      <c r="C74" s="75"/>
-      <c r="D74" s="93"/>
-      <c r="E74" s="89" t="s">
+      <c r="A74" s="55"/>
+      <c r="B74" s="55"/>
+      <c r="C74" s="55"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F74" s="78"/>
-      <c r="G74" s="79"/>
-      <c r="H74" s="79"/>
-      <c r="I74" s="75"/>
-      <c r="J74" s="75"/>
+      <c r="F74" s="80"/>
+      <c r="G74" s="60"/>
+      <c r="H74" s="60"/>
+      <c r="I74" s="55"/>
+      <c r="J74" s="55"/>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A75" s="75"/>
-      <c r="B75" s="75"/>
-      <c r="C75" s="75"/>
-      <c r="D75" s="93"/>
+      <c r="A75" s="55"/>
+      <c r="B75" s="55"/>
+      <c r="C75" s="55"/>
+      <c r="D75" s="67"/>
       <c r="E75" s="28" t="s">
         <v>65</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="20"/>
-      <c r="H75" s="79"/>
-      <c r="I75" s="75"/>
-      <c r="J75" s="75"/>
+      <c r="H75" s="60"/>
+      <c r="I75" s="55"/>
+      <c r="J75" s="55"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A76" s="75"/>
-      <c r="B76" s="75"/>
-      <c r="C76" s="75"/>
-      <c r="D76" s="93"/>
+      <c r="A76" s="55"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="67"/>
       <c r="E76" s="28" t="s">
         <v>78</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="20"/>
-      <c r="H76" s="79"/>
-      <c r="I76" s="75"/>
-      <c r="J76" s="75"/>
+      <c r="H76" s="60"/>
+      <c r="I76" s="55"/>
+      <c r="J76" s="55"/>
     </row>
     <row r="77" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A77" s="75"/>
-      <c r="B77" s="75"/>
-      <c r="C77" s="75"/>
-      <c r="D77" s="93"/>
+      <c r="A77" s="55"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="55"/>
+      <c r="D77" s="67"/>
       <c r="E77" s="28"/>
       <c r="F77" s="9"/>
       <c r="G77" s="20"/>
-      <c r="H77" s="79"/>
-      <c r="I77" s="75"/>
-      <c r="J77" s="75"/>
+      <c r="H77" s="60"/>
+      <c r="I77" s="55"/>
+      <c r="J77" s="55"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A78" s="75"/>
-      <c r="B78" s="76"/>
-      <c r="C78" s="76"/>
-      <c r="D78" s="70"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="34"/>
-      <c r="H78" s="72"/>
-      <c r="I78" s="76"/>
-      <c r="J78" s="76"/>
+      <c r="A78" s="55"/>
+      <c r="B78" s="56"/>
+      <c r="C78" s="56"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="61"/>
+      <c r="I78" s="56"/>
+      <c r="J78" s="56"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A79" s="75"/>
-      <c r="B79" s="90" t="s">
+      <c r="A79" s="55"/>
+      <c r="B79" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C79" s="91" t="s">
+      <c r="C79" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="D79" s="92" t="s">
+      <c r="D79" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="E79" s="88" t="s">
+      <c r="E79" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="F79" s="68"/>
-      <c r="G79" s="69"/>
-      <c r="H79" s="98" t="s">
+      <c r="F79" s="76"/>
+      <c r="G79" s="75"/>
+      <c r="H79" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="I79" s="96" t="s">
+      <c r="I79" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="J79" s="97" t="s">
+      <c r="J79" s="57" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A80" s="75"/>
-      <c r="B80" s="75"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="93"/>
-      <c r="E80" s="89" t="s">
+      <c r="A80" s="55"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="55"/>
+      <c r="D80" s="67"/>
+      <c r="E80" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F80" s="78"/>
-      <c r="G80" s="79"/>
-      <c r="H80" s="79"/>
-      <c r="I80" s="75"/>
-      <c r="J80" s="75"/>
+      <c r="F80" s="80"/>
+      <c r="G80" s="60"/>
+      <c r="H80" s="60"/>
+      <c r="I80" s="55"/>
+      <c r="J80" s="55"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A81" s="75"/>
-      <c r="B81" s="75"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="93"/>
+      <c r="A81" s="55"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="55"/>
+      <c r="D81" s="67"/>
       <c r="E81" s="28" t="s">
         <v>70</v>
       </c>
       <c r="F81" s="9"/>
       <c r="G81" s="20"/>
-      <c r="H81" s="79"/>
-      <c r="I81" s="75"/>
-      <c r="J81" s="75"/>
+      <c r="H81" s="60"/>
+      <c r="I81" s="55"/>
+      <c r="J81" s="55"/>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A82" s="75"/>
-      <c r="B82" s="75"/>
-      <c r="C82" s="75"/>
-      <c r="D82" s="93"/>
+      <c r="A82" s="55"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="55"/>
+      <c r="D82" s="67"/>
       <c r="E82" s="28" t="s">
         <v>66</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="20"/>
-      <c r="H82" s="79"/>
-      <c r="I82" s="75"/>
-      <c r="J82" s="75"/>
+      <c r="H82" s="60"/>
+      <c r="I82" s="55"/>
+      <c r="J82" s="55"/>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A83" s="75"/>
-      <c r="B83" s="75"/>
-      <c r="C83" s="75"/>
-      <c r="D83" s="93"/>
+      <c r="A83" s="55"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="55"/>
+      <c r="D83" s="67"/>
       <c r="E83" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F83" s="9"/>
       <c r="G83" s="20"/>
-      <c r="H83" s="79"/>
-      <c r="I83" s="75"/>
-      <c r="J83" s="75"/>
+      <c r="H83" s="60"/>
+      <c r="I83" s="55"/>
+      <c r="J83" s="55"/>
     </row>
     <row r="84" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A84" s="76"/>
-      <c r="B84" s="76"/>
-      <c r="C84" s="76"/>
-      <c r="D84" s="70"/>
+      <c r="A84" s="56"/>
+      <c r="B84" s="56"/>
+      <c r="C84" s="56"/>
+      <c r="D84" s="68"/>
       <c r="E84" s="29" t="s">
         <v>68</v>
       </c>
       <c r="F84" s="22"/>
       <c r="G84" s="23"/>
-      <c r="H84" s="72"/>
-      <c r="I84" s="76"/>
-      <c r="J84" s="76"/>
+      <c r="H84" s="61"/>
+      <c r="I84" s="56"/>
+      <c r="J84" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="130">
-    <mergeCell ref="I55:I60"/>
-    <mergeCell ref="J55:J60"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="H49:H54"/>
-    <mergeCell ref="I49:I54"/>
-    <mergeCell ref="J49:J54"/>
-    <mergeCell ref="H55:H60"/>
+  <mergeCells count="138">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="E12:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="J26:J29"/>
+    <mergeCell ref="J30:J33"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="J22:J25"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="I26:I29"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="J34:J37"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="B61:B66"/>
+    <mergeCell ref="C61:C66"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="C67:C72"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="A14:A45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="C79:C84"/>
+    <mergeCell ref="D79:D84"/>
+    <mergeCell ref="A49:A84"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="D49:D54"/>
+    <mergeCell ref="D61:D66"/>
+    <mergeCell ref="C55:C60"/>
+    <mergeCell ref="D55:D60"/>
     <mergeCell ref="I42:I45"/>
     <mergeCell ref="J42:J45"/>
     <mergeCell ref="H38:H41"/>
@@ -3092,109 +3230,15 @@
     <mergeCell ref="I67:I72"/>
     <mergeCell ref="J67:J72"/>
     <mergeCell ref="H73:H78"/>
-    <mergeCell ref="D73:D78"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="C79:C84"/>
-    <mergeCell ref="D79:D84"/>
-    <mergeCell ref="A49:A84"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C49:C54"/>
-    <mergeCell ref="D49:D54"/>
-    <mergeCell ref="D61:D66"/>
-    <mergeCell ref="C55:C60"/>
-    <mergeCell ref="D55:D60"/>
-    <mergeCell ref="A14:A45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="B61:B66"/>
-    <mergeCell ref="C61:C66"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="C67:C72"/>
-    <mergeCell ref="D67:D72"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="J26:J29"/>
-    <mergeCell ref="J30:J33"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="J22:J25"/>
-    <mergeCell ref="I22:I25"/>
-    <mergeCell ref="I26:I29"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I34:I37"/>
-    <mergeCell ref="J34:J37"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E12:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I14:I17"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I55:I60"/>
+    <mergeCell ref="J55:J60"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="H49:H54"/>
+    <mergeCell ref="I49:I54"/>
+    <mergeCell ref="J49:J54"/>
+    <mergeCell ref="H55:H60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1"/>
@@ -3233,1208 +3277,1254 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="108" t="s">
+      <c r="E2" s="85"/>
+      <c r="F2" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="58"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="91"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="38" t="s">
+      <c r="B3" s="85"/>
+      <c r="C3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="D3" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="55"/>
+      <c r="E3" s="85"/>
       <c r="F3" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="110" t="s">
+      <c r="G3" s="91"/>
+      <c r="H3" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="111" t="s">
+      <c r="I3" s="100"/>
+      <c r="J3" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="58"/>
+      <c r="K3" s="91"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="55"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="109"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="85"/>
+      <c r="C7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="107" t="s">
+      <c r="D7" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="113">
+      <c r="E7" s="85"/>
+      <c r="F7" s="110">
         <v>44985</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="114" t="s">
+      <c r="G7" s="91"/>
+      <c r="H7" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="115" t="s">
+      <c r="I7" s="85"/>
+      <c r="J7" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="58"/>
+      <c r="K7" s="91"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="81" t="s">
+      <c r="C9" s="76"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="68"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="81" t="s">
+      <c r="G9" s="76"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="81" t="s">
+      <c r="K9" s="87" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="76"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="74" t="s">
+      <c r="C11" s="75"/>
+      <c r="D11" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="116" t="s">
+      <c r="E11" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="F11" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="102" t="s">
+      <c r="G11" s="41"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="100" t="s">
+      <c r="J11" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="82" t="s">
+      <c r="K11" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="75"/>
-      <c r="B12" s="93"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="44" t="s">
+      <c r="A12" s="55"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="75"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="44" t="s">
+      <c r="A13" s="55"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="75"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="44" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="75"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="44" t="s">
+      <c r="A15" s="55"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A16" s="75"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="44" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="75"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="44" t="s">
+      <c r="A17" s="55"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="75"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="46" t="s">
+      <c r="A18" s="55"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A19" s="75"/>
-      <c r="B19" s="101" t="s">
+      <c r="A19" s="55"/>
+      <c r="B19" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="74" t="s">
+      <c r="C19" s="75"/>
+      <c r="D19" s="64" t="s">
         <v>96</v>
       </c>
       <c r="E19" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="F19" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="80" t="s">
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="J19" s="100" t="s">
+      <c r="J19" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="82" t="s">
+      <c r="K19" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="75"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="44" t="s">
+      <c r="A20" s="55"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="75"/>
-      <c r="B21" s="93"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="44" t="s">
+      <c r="A21" s="55"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="75"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="75"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="75"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="75"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="75"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="75"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="76"/>
-      <c r="K26" s="76"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="75"/>
-      <c r="B27" s="101" t="s">
+      <c r="A27" s="55"/>
+      <c r="B27" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="74" t="s">
+      <c r="C27" s="75"/>
+      <c r="D27" s="64" t="s">
         <v>100</v>
       </c>
       <c r="E27" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="80" t="s">
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="J27" s="100" t="s">
+      <c r="J27" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="82" t="s">
+      <c r="K27" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="75"/>
-      <c r="B28" s="93"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="44" t="s">
+      <c r="A28" s="55"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="75"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="75"/>
-      <c r="B29" s="93"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="44" t="s">
+      <c r="A29" s="55"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="75"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="79"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="44" t="s">
+      <c r="A30" s="55"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="75"/>
-      <c r="B31" s="93"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="44" t="s">
+      <c r="A31" s="55"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="36"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="75"/>
-      <c r="B32" s="93"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="44" t="s">
+      <c r="A32" s="55"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="75"/>
-      <c r="B33" s="93"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="44" t="s">
+      <c r="A33" s="55"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="75"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="75"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="46" t="s">
+      <c r="A34" s="55"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="76"/>
-      <c r="K34" s="76"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="75"/>
-      <c r="B35" s="101" t="s">
+      <c r="A35" s="55"/>
+      <c r="B35" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="69"/>
-      <c r="D35" s="74" t="s">
+      <c r="C35" s="75"/>
+      <c r="D35" s="64" t="s">
         <v>103</v>
       </c>
       <c r="E35" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="41" t="s">
+      <c r="F35" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G35" s="42"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="80" t="s">
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="J35" s="100" t="s">
+      <c r="J35" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K35" s="82" t="s">
+      <c r="K35" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="75"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="44" t="s">
+      <c r="A36" s="55"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="75"/>
-      <c r="J36" s="75"/>
-      <c r="K36" s="75"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="75"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="44" t="s">
+      <c r="A37" s="55"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="75"/>
-      <c r="K37" s="75"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="75"/>
-      <c r="B38" s="93"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="49" t="s">
+      <c r="A38" s="55"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="75"/>
-      <c r="J38" s="75"/>
-      <c r="K38" s="75"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="75"/>
-      <c r="B39" s="93"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="75"/>
-      <c r="F39" s="44" t="s">
+      <c r="A39" s="55"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="75"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="75"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A40" s="75"/>
-      <c r="B40" s="93"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="44" t="s">
+      <c r="A40" s="55"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="G40" s="36"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="75"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A41" s="75"/>
-      <c r="B41" s="93"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="44" t="s">
+      <c r="A41" s="55"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="G41" s="36"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="75"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="46" t="s">
+      <c r="A42" s="55"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="G42" s="47"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="76"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="75"/>
-      <c r="B43" s="101" t="s">
+      <c r="A43" s="55"/>
+      <c r="B43" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="69"/>
-      <c r="D43" s="74" t="s">
+      <c r="C43" s="75"/>
+      <c r="D43" s="64" t="s">
         <v>107</v>
       </c>
       <c r="E43" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="F43" s="41" t="s">
+      <c r="F43" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G43" s="42"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="80" t="s">
+      <c r="G43" s="41"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="J43" s="100" t="s">
+      <c r="J43" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K43" s="82" t="s">
+      <c r="K43" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="75"/>
-      <c r="B44" s="93"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="44" t="s">
+      <c r="A44" s="55"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="G44" s="36"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="75"/>
-      <c r="J44" s="75"/>
-      <c r="K44" s="75"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A45" s="75"/>
-      <c r="B45" s="93"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="44" t="s">
+      <c r="A45" s="55"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="G45" s="36"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="75"/>
-      <c r="J45" s="75"/>
-      <c r="K45" s="75"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A46" s="75"/>
-      <c r="B46" s="93"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="49" t="s">
+      <c r="A46" s="55"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="G46" s="36"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="75"/>
-      <c r="J46" s="75"/>
-      <c r="K46" s="75"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="55"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="75"/>
-      <c r="B47" s="93"/>
-      <c r="C47" s="79"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="44" t="s">
+      <c r="A47" s="55"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="G47" s="36"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="75"/>
-      <c r="J47" s="75"/>
-      <c r="K47" s="75"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A48" s="75"/>
-      <c r="B48" s="93"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="44" t="s">
+      <c r="A48" s="55"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="G48" s="36"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="75"/>
-      <c r="J48" s="75"/>
-      <c r="K48" s="75"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A49" s="75"/>
-      <c r="B49" s="93"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="44" t="s">
+      <c r="A49" s="55"/>
+      <c r="B49" s="67"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="G49" s="36"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="75"/>
-      <c r="J49" s="75"/>
-      <c r="K49" s="75"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="55"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="55"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A50" s="75"/>
-      <c r="B50" s="70"/>
-      <c r="C50" s="72"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="76"/>
-      <c r="F50" s="46" t="s">
+      <c r="A50" s="55"/>
+      <c r="B50" s="68"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="G50" s="47"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="76"/>
-      <c r="J50" s="76"/>
-      <c r="K50" s="76"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A51" s="75"/>
-      <c r="B51" s="101" t="s">
+      <c r="A51" s="55"/>
+      <c r="B51" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="74" t="s">
+      <c r="C51" s="75"/>
+      <c r="D51" s="64" t="s">
         <v>111</v>
       </c>
       <c r="E51" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="F51" s="41" t="s">
+      <c r="F51" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G51" s="42"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="80" t="s">
+      <c r="G51" s="41"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="J51" s="100" t="s">
+      <c r="J51" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K51" s="82" t="s">
+      <c r="K51" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A52" s="75"/>
-      <c r="B52" s="93"/>
-      <c r="C52" s="79"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="44" t="s">
+      <c r="A52" s="55"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="36"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="75"/>
-      <c r="J52" s="75"/>
-      <c r="K52" s="75"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="55"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="55"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A53" s="75"/>
-      <c r="B53" s="93"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="44" t="s">
+      <c r="A53" s="55"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="G53" s="36"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="75"/>
-      <c r="J53" s="75"/>
-      <c r="K53" s="75"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="55"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A54" s="75"/>
-      <c r="B54" s="93"/>
-      <c r="C54" s="79"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="49" t="s">
+      <c r="A54" s="55"/>
+      <c r="B54" s="67"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="G54" s="36"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="75"/>
-      <c r="J54" s="75"/>
-      <c r="K54" s="75"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="55"/>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A55" s="75"/>
-      <c r="B55" s="93"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="44" t="s">
+      <c r="A55" s="55"/>
+      <c r="B55" s="67"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="G55" s="36"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="75"/>
-      <c r="J55" s="75"/>
-      <c r="K55" s="75"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="55"/>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A56" s="75"/>
-      <c r="B56" s="93"/>
-      <c r="C56" s="79"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="44" t="s">
+      <c r="A56" s="55"/>
+      <c r="B56" s="67"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="G56" s="36"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="75"/>
-      <c r="J56" s="75"/>
-      <c r="K56" s="75"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="55"/>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A57" s="75"/>
-      <c r="B57" s="93"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
-      <c r="K57" s="75"/>
+      <c r="A57" s="55"/>
+      <c r="B57" s="67"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="55"/>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A58" s="76"/>
-      <c r="B58" s="70"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="76"/>
-      <c r="E58" s="76"/>
-      <c r="F58" s="46"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="76"/>
-      <c r="J58" s="76"/>
-      <c r="K58" s="76"/>
+      <c r="A58" s="56"/>
+      <c r="B58" s="68"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="56"/>
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A59" s="50"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="50"/>
+      <c r="A59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A60" s="81" t="s">
+      <c r="A60" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="67" t="s">
+      <c r="B60" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="68"/>
-      <c r="D60" s="69"/>
-      <c r="E60" s="81" t="s">
+      <c r="C60" s="76"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="F60" s="67" t="s">
+      <c r="F60" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="G60" s="68"/>
-      <c r="H60" s="69"/>
-      <c r="I60" s="81" t="s">
+      <c r="G60" s="76"/>
+      <c r="H60" s="75"/>
+      <c r="I60" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="J60" s="81" t="s">
+      <c r="J60" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="K60" s="81" t="s">
+      <c r="K60" s="87" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A61" s="76"/>
-      <c r="B61" s="70"/>
-      <c r="C61" s="71"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="70"/>
-      <c r="G61" s="71"/>
-      <c r="H61" s="72"/>
-      <c r="I61" s="76"/>
-      <c r="J61" s="76"/>
-      <c r="K61" s="76"/>
+      <c r="A61" s="56"/>
+      <c r="B61" s="68"/>
+      <c r="C61" s="77"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="68"/>
+      <c r="G61" s="77"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="56"/>
+      <c r="J61" s="56"/>
+      <c r="K61" s="56"/>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1">
       <c r="A62" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="B62" s="101" t="s">
+      <c r="B62" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="69"/>
-      <c r="D62" s="74" t="s">
+      <c r="C62" s="75"/>
+      <c r="D62" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="E62" s="105" t="s">
+      <c r="E62" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="F62" s="41" t="s">
+      <c r="F62" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="G62" s="42"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="102" t="s">
+      <c r="G62" s="41"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="J62" s="80" t="s">
+      <c r="J62" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="K62" s="103" t="s">
+      <c r="K62" s="117" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A63" s="75"/>
-      <c r="B63" s="93"/>
-      <c r="C63" s="79"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="93"/>
-      <c r="F63" s="44" t="s">
+      <c r="A63" s="55"/>
+      <c r="B63" s="67"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="67"/>
+      <c r="F63" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="G63" s="36"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="79"/>
-      <c r="J63" s="75"/>
-      <c r="K63" s="75"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="60"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="55"/>
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A64" s="75"/>
-      <c r="B64" s="93"/>
-      <c r="C64" s="79"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="93"/>
-      <c r="F64" s="44" t="s">
+      <c r="A64" s="55"/>
+      <c r="B64" s="67"/>
+      <c r="C64" s="60"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G64" s="36"/>
-      <c r="H64" s="45"/>
-      <c r="I64" s="79"/>
-      <c r="J64" s="75"/>
-      <c r="K64" s="75"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="44"/>
+      <c r="I64" s="60"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="55"/>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A65" s="75"/>
-      <c r="B65" s="93"/>
-      <c r="C65" s="79"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="93"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="45"/>
-      <c r="I65" s="79"/>
-      <c r="J65" s="75"/>
-      <c r="K65" s="75"/>
+      <c r="A65" s="55"/>
+      <c r="B65" s="67"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="55"/>
+      <c r="E65" s="67"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="60"/>
+      <c r="J65" s="55"/>
+      <c r="K65" s="55"/>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A66" s="76"/>
-      <c r="B66" s="70"/>
-      <c r="C66" s="72"/>
-      <c r="D66" s="76"/>
-      <c r="E66" s="70"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="33"/>
-      <c r="H66" s="34"/>
-      <c r="I66" s="72"/>
-      <c r="J66" s="76"/>
-      <c r="K66" s="76"/>
+      <c r="A66" s="56"/>
+      <c r="B66" s="68"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="61"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="56"/>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A68" s="81" t="s">
+      <c r="A68" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B68" s="67" t="s">
+      <c r="B68" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="68"/>
-      <c r="D68" s="69"/>
-      <c r="E68" s="81" t="s">
+      <c r="C68" s="76"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="F68" s="67" t="s">
+      <c r="F68" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="G68" s="68"/>
-      <c r="H68" s="69"/>
-      <c r="I68" s="81" t="s">
+      <c r="G68" s="76"/>
+      <c r="H68" s="75"/>
+      <c r="I68" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="J68" s="81" t="s">
+      <c r="J68" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="K68" s="81" t="s">
+      <c r="K68" s="87" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A69" s="76"/>
-      <c r="B69" s="70"/>
-      <c r="C69" s="71"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="76"/>
-      <c r="F69" s="70"/>
-      <c r="G69" s="71"/>
-      <c r="H69" s="72"/>
-      <c r="I69" s="76"/>
-      <c r="J69" s="76"/>
-      <c r="K69" s="76"/>
+      <c r="A69" s="56"/>
+      <c r="B69" s="68"/>
+      <c r="C69" s="77"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="77"/>
+      <c r="H69" s="61"/>
+      <c r="I69" s="56"/>
+      <c r="J69" s="56"/>
+      <c r="K69" s="56"/>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1">
       <c r="A70" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="B70" s="104" t="s">
+      <c r="B70" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="69"/>
-      <c r="D70" s="74" t="s">
+      <c r="C70" s="75"/>
+      <c r="D70" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="E70" s="105" t="s">
+      <c r="E70" s="116" t="s">
         <v>121</v>
       </c>
       <c r="F70" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="G70" s="51"/>
-      <c r="H70" s="52"/>
-      <c r="I70" s="106" t="s">
+      <c r="G70" s="50"/>
+      <c r="H70" s="51"/>
+      <c r="I70" s="118" t="s">
         <v>123</v>
       </c>
-      <c r="J70" s="80" t="s">
+      <c r="J70" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="K70" s="103" t="s">
+      <c r="K70" s="117" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A71" s="75"/>
-      <c r="B71" s="93"/>
-      <c r="C71" s="79"/>
-      <c r="D71" s="75"/>
-      <c r="E71" s="93"/>
-      <c r="F71" s="53"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="75"/>
-      <c r="J71" s="75"/>
-      <c r="K71" s="75"/>
+      <c r="A71" s="55"/>
+      <c r="B71" s="67"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="67"/>
+      <c r="F71" s="52"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="55"/>
+      <c r="J71" s="55"/>
+      <c r="K71" s="55"/>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A72" s="76"/>
-      <c r="B72" s="70"/>
-      <c r="C72" s="72"/>
-      <c r="D72" s="76"/>
-      <c r="E72" s="70"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="33"/>
-      <c r="H72" s="34"/>
-      <c r="I72" s="76"/>
-      <c r="J72" s="76"/>
-      <c r="K72" s="76"/>
+      <c r="A72" s="56"/>
+      <c r="B72" s="68"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="56"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="33"/>
+      <c r="I72" s="56"/>
+      <c r="J72" s="56"/>
+      <c r="K72" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B11:C18"/>
-    <mergeCell ref="D11:D18"/>
-    <mergeCell ref="E11:E18"/>
-    <mergeCell ref="B19:C26"/>
+    <mergeCell ref="I35:I42"/>
+    <mergeCell ref="I43:I50"/>
+    <mergeCell ref="J43:J50"/>
+    <mergeCell ref="K43:K50"/>
+    <mergeCell ref="I19:I26"/>
+    <mergeCell ref="J19:J26"/>
+    <mergeCell ref="I27:I34"/>
+    <mergeCell ref="J27:J34"/>
+    <mergeCell ref="K27:K34"/>
+    <mergeCell ref="J35:J42"/>
+    <mergeCell ref="K35:K42"/>
+    <mergeCell ref="D19:D26"/>
+    <mergeCell ref="E19:E26"/>
+    <mergeCell ref="B27:C34"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="E27:E34"/>
+    <mergeCell ref="E35:E42"/>
+    <mergeCell ref="B35:C42"/>
+    <mergeCell ref="B43:C50"/>
+    <mergeCell ref="D43:D50"/>
+    <mergeCell ref="E43:E50"/>
+    <mergeCell ref="J62:J66"/>
+    <mergeCell ref="B60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="J70:J72"/>
+    <mergeCell ref="K70:K72"/>
+    <mergeCell ref="I70:I72"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="B62:C66"/>
+    <mergeCell ref="K62:K66"/>
+    <mergeCell ref="F60:H61"/>
+    <mergeCell ref="B68:D69"/>
+    <mergeCell ref="D62:D66"/>
+    <mergeCell ref="E62:E66"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="F68:H69"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A58"/>
@@ -4451,68 +4541,22 @@
     <mergeCell ref="I51:I58"/>
     <mergeCell ref="J51:J58"/>
     <mergeCell ref="K51:K58"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B11:C18"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="E11:E18"/>
+    <mergeCell ref="B19:C26"/>
     <mergeCell ref="B70:C72"/>
     <mergeCell ref="D70:D72"/>
     <mergeCell ref="E70:E72"/>
-    <mergeCell ref="J70:J72"/>
-    <mergeCell ref="K70:K72"/>
-    <mergeCell ref="I70:I72"/>
-    <mergeCell ref="K60:K61"/>
-    <mergeCell ref="B62:C66"/>
-    <mergeCell ref="K62:K66"/>
-    <mergeCell ref="F60:H61"/>
-    <mergeCell ref="B68:D69"/>
-    <mergeCell ref="D62:D66"/>
-    <mergeCell ref="E62:E66"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="K68:K69"/>
-    <mergeCell ref="F68:H69"/>
-    <mergeCell ref="J68:J69"/>
     <mergeCell ref="B51:C58"/>
     <mergeCell ref="D51:D58"/>
     <mergeCell ref="E51:E58"/>
-    <mergeCell ref="I62:I66"/>
-    <mergeCell ref="J62:J66"/>
-    <mergeCell ref="B60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="J60:J61"/>
     <mergeCell ref="D35:D42"/>
-    <mergeCell ref="E35:E42"/>
-    <mergeCell ref="B35:C42"/>
-    <mergeCell ref="B43:C50"/>
-    <mergeCell ref="D43:D50"/>
-    <mergeCell ref="E43:E50"/>
-    <mergeCell ref="D19:D26"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="B27:C34"/>
-    <mergeCell ref="D27:D34"/>
-    <mergeCell ref="E27:E34"/>
-    <mergeCell ref="I35:I42"/>
-    <mergeCell ref="I43:I50"/>
-    <mergeCell ref="J43:J50"/>
-    <mergeCell ref="K43:K50"/>
-    <mergeCell ref="I19:I26"/>
-    <mergeCell ref="J19:J26"/>
-    <mergeCell ref="I27:I34"/>
-    <mergeCell ref="J27:J34"/>
-    <mergeCell ref="K27:K34"/>
-    <mergeCell ref="J35:J42"/>
-    <mergeCell ref="K35:K42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>

</xml_diff>